<commit_message>
FEW MORE TEMPLATE UPDATED
</commit_message>
<xml_diff>
--- a/Insurance/insurance_templates/arabia.xlsx
+++ b/Insurance/insurance_templates/arabia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\algaeh-monorepo\Insurance\insurance_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C116325-6323-463A-87CB-07B9FFB8ACDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71607815-5C9C-470A-AC44-BBA523A62B16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
     <t>Policy Holder:-</t>
   </si>
   <si>
-    <t>MEDGULF TAKAFUL</t>
+    <t>ARBIA</t>
   </si>
 </sst>
 </file>
@@ -227,14 +227,32 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -245,38 +263,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -539,7 +539,7 @@
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="J3" sqref="J3:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -559,31 +559,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="6" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
     </row>
-    <row r="2" spans="1:15" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:15" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
       <c r="E2" s="7" t="s">
         <v>15</v>
       </c>
@@ -601,74 +601,74 @@
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="11" t="s">
+      <c r="F3" s="15"/>
+      <c r="G3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="14" t="s">
+      <c r="H3" s="14"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="16"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>